<commit_message>
adding results, standings, assist network...
</commit_message>
<xml_diff>
--- a/data/xlsx/2020-24.xlsx
+++ b/data/xlsx/2020-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/github/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C39E39-9CC7-FB44-A541-822B3AC36BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1439D415-F418-7D4B-81DD-C1DD46BE4241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="122">
   <si>
     <t>team</t>
   </si>
@@ -86,9 +86,6 @@
     <t>John Lemen</t>
   </si>
   <si>
-    <t>Daniel Negron</t>
-  </si>
-  <si>
     <t>David Laux</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Bill Oehlschlager</t>
   </si>
   <si>
-    <t>Brett A Schneider</t>
-  </si>
-  <si>
     <t>Brian Lin</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>Aaron Vivian</t>
   </si>
   <si>
-    <t>Brett J Schneider</t>
-  </si>
-  <si>
     <t>Katy McVay</t>
   </si>
   <si>
@@ -408,6 +399,9 @@
   </si>
   <si>
     <t>Team Gold</t>
+  </si>
+  <si>
+    <t>Brett Schneider (Bort)</t>
   </si>
 </sst>
 </file>
@@ -793,7 +787,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -807,7 +801,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -821,7 +815,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -835,7 +829,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -856,7 +850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B76DB8F-6AF4-5346-B458-3D7F7E4A99E1}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -882,10 +878,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -893,41 +889,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -935,105 +931,105 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1042,49 +1038,49 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1092,13 +1088,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1110,7 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46413781-6423-5D42-B78C-D1E073E91648}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1122,24 +1118,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -1148,466 +1144,466 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="I19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1630,24 +1626,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -1656,32 +1652,32 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1693,391 +1689,391 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="I16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed game result calculation, update database, added some helper scripts...
</commit_message>
<xml_diff>
--- a/data/xlsx/2020-24.xlsx
+++ b/data/xlsx/2020-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/github/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1439D415-F418-7D4B-81DD-C1DD46BE4241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E839A535-5A10-424B-AE8B-A1560B3DC86E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="122">
   <si>
     <t>team</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Patrick Joyce</t>
   </si>
   <si>
-    <t>Aaron Bill</t>
-  </si>
-  <si>
     <t>Benny Docter</t>
   </si>
   <si>
@@ -402,6 +399,9 @@
   </si>
   <si>
     <t>Brett Schneider (Bort)</t>
+  </si>
+  <si>
+    <t>Luke Bill</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B76DB8F-6AF4-5346-B458-3D7F7E4A99E1}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,10 +878,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -889,16 +889,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -906,13 +906,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -920,10 +920,10 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -934,13 +934,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -948,13 +948,13 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -962,13 +962,13 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -976,13 +976,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -993,10 +993,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1004,13 +1004,13 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1018,13 +1018,13 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1038,7 +1038,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1046,13 +1046,13 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1060,13 +1060,13 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1074,13 +1074,13 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1088,13 +1088,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46413781-6423-5D42-B78C-D1E073E91648}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1118,24 +1118,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -1144,41 +1144,41 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>28</v>
@@ -1186,74 +1186,74 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>27</v>
@@ -1262,132 +1262,132 @@
         <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1399,129 +1399,129 @@
         <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>23</v>
@@ -1533,77 +1533,77 @@
         <v>26</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1616,7 +1616,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1626,24 +1626,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -1652,32 +1652,32 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1689,391 +1689,394 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="I17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="I18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using 0 to denote unknown period, also database update...
</commit_message>
<xml_diff>
--- a/data/xlsx/2020-24.xlsx
+++ b/data/xlsx/2020-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/github/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A466E353-F963-D043-8A61-D4A68754F07B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D96E26-7C3C-9F49-9B29-9EB18A5B995E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="5" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="7" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="1-2" sheetId="4" r:id="rId4"/>
     <sheet name="2-1" sheetId="5" r:id="rId5"/>
     <sheet name="2-2" sheetId="6" r:id="rId6"/>
+    <sheet name="3-1" sheetId="7" r:id="rId7"/>
+    <sheet name="3-2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="179">
   <si>
     <t>team</t>
   </si>
@@ -500,6 +502,81 @@
   </si>
   <si>
     <t>02:07</t>
+  </si>
+  <si>
+    <t>2019-02-23</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>Hooking</t>
+  </si>
+  <si>
+    <t>05:20</t>
+  </si>
+  <si>
+    <t>04:22</t>
+  </si>
+  <si>
+    <t>01:24</t>
+  </si>
+  <si>
+    <t>11:15</t>
+  </si>
+  <si>
+    <t>01:08</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>19:45</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>16:30</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>09:30</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>01:20</t>
+  </si>
+  <si>
+    <t>00:55</t>
+  </si>
+  <si>
+    <t>Unsportsmanlike Conduct</t>
+  </si>
+  <si>
+    <t>High Sticking</t>
+  </si>
+  <si>
+    <t>03:45</t>
   </si>
 </sst>
 </file>
@@ -548,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -558,6 +635,10 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,7 +1050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B76DB8F-6AF4-5346-B458-3D7F7E4A99E1}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2704,7 +2787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E664A11-AA1D-1748-8E47-B783357EB18B}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3265,4 +3348,1042 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D6BA78-F449-744C-AE19-18F147C0B270}">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5BE2C1-9760-C343-8BDC-E0A825E35D77}">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor and update deprecated/retired tidyverse functions
</commit_message>
<xml_diff>
--- a/data/xlsx/2020-24.xlsx
+++ b/data/xlsx/2020-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnanto/GitHub/broomball/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911C07D4-91A6-D948-96E1-0D1BA77BB3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AD5BB3-46D4-7649-B94C-9696D9ADD5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="4" xr2:uid="{2B2C1B60-C7C7-204A-B366-650A95809B61}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="180">
   <si>
     <t>team</t>
   </si>
@@ -321,9 +321,6 @@
     <t>The St. James</t>
   </si>
   <si>
-    <t>2019-01-26</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>Luke Bill</t>
   </si>
   <si>
-    <t>2019-02-14</t>
-  </si>
-  <si>
     <t>Sean Greeney</t>
   </si>
   <si>
@@ -504,9 +498,6 @@
     <t>02:07</t>
   </si>
   <si>
-    <t>2019-02-23</t>
-  </si>
-  <si>
     <t>16:00</t>
   </si>
   <si>
@@ -577,6 +568,18 @@
   </si>
   <si>
     <t>03:45</t>
+  </si>
+  <si>
+    <t>2020-01-26</t>
+  </si>
+  <si>
+    <t>2020-02-14</t>
+  </si>
+  <si>
+    <t>2020-02-23</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -979,7 +982,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -993,7 +996,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1007,7 +1010,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1035,10 +1038,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1050,9 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B76DB8F-6AF4-5346-B458-3D7F7E4A99E1}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1073,7 +1074,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1081,7 +1082,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -1090,12 +1091,12 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -1104,7 +1105,7 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1154,10 +1155,10 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -1312,9 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46413781-6423-5D42-B78C-D1E073E91648}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1350,7 +1349,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -1381,10 +1380,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>28</v>
@@ -1398,10 +1397,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>40</v>
@@ -1456,10 +1455,10 @@
         <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>27</v>
@@ -1474,13 +1473,13 @@
         <v>73</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1506,13 +1505,13 @@
         <v>73</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1526,7 +1525,7 @@
         <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>30</v>
@@ -1538,13 +1537,13 @@
         <v>73</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1573,13 +1572,13 @@
         <v>73</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1593,7 +1592,7 @@
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1611,13 +1610,13 @@
         <v>73</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1640,13 +1639,13 @@
         <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1660,7 +1659,7 @@
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>30</v>
@@ -1672,13 +1671,13 @@
         <v>73</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1692,7 +1691,7 @@
         <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
@@ -1707,13 +1706,13 @@
         <v>73</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1727,7 +1726,7 @@
         <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>23</v>
@@ -1745,13 +1744,13 @@
         <v>73</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1797,10 +1796,10 @@
         <v>74</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>74</v>
@@ -1809,7 +1808,7 @@
         <v>28</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +1855,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -1904,10 +1903,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>66</v>
@@ -1971,16 +1970,16 @@
         <v>53</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>73</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1994,10 +1993,10 @@
         <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>52</v>
@@ -2009,13 +2008,13 @@
         <v>73</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2029,7 +2028,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>48</v>
@@ -2041,16 +2040,16 @@
         <v>66</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2064,13 +2063,13 @@
         <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
@@ -2082,13 +2081,13 @@
         <v>73</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -2102,7 +2101,7 @@
         <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>65</v>
@@ -2117,13 +2116,13 @@
         <v>73</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2137,7 +2136,7 @@
         <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
@@ -2155,13 +2154,13 @@
         <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -2207,13 +2206,13 @@
         <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>74</v>
@@ -2236,13 +2235,13 @@
         <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>58</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>74</v>
@@ -2265,13 +2264,13 @@
         <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>74</v>
@@ -2280,7 +2279,7 @@
         <v>53</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2292,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2329,7 +2328,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -2361,7 +2360,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>48</v>
@@ -2375,13 +2374,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2392,10 +2391,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
@@ -2450,7 +2449,7 @@
         <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>33</v>
@@ -2465,13 +2464,13 @@
         <v>73</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2485,7 +2484,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -2494,19 +2493,19 @@
         <v>35</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2520,7 +2519,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>48</v>
@@ -2532,16 +2531,16 @@
         <v>8</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2555,25 +2554,25 @@
         <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>73</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2587,10 +2586,10 @@
         <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>52</v>
@@ -2602,13 +2601,13 @@
         <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2655,13 +2654,13 @@
         <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>74</v>
@@ -2670,7 +2669,7 @@
         <v>8</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2684,13 +2683,13 @@
         <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>74</v>
@@ -2713,27 +2712,27 @@
         <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>77</v>
@@ -2742,36 +2741,36 @@
         <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>75</v>
@@ -2821,7 +2820,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -2853,10 +2852,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>28</v>
@@ -2870,10 +2869,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>66</v>
@@ -2928,13 +2927,13 @@
         <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>30</v>
@@ -2946,13 +2945,13 @@
         <v>73</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -2966,7 +2965,7 @@
         <v>73</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -2984,13 +2983,13 @@
         <v>73</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3004,7 +3003,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -3022,13 +3021,13 @@
         <v>73</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3042,7 +3041,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>60</v>
@@ -3060,13 +3059,13 @@
         <v>73</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3080,7 +3079,7 @@
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>58</v>
@@ -3095,13 +3094,13 @@
         <v>73</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3115,7 +3114,7 @@
         <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>7</v>
@@ -3130,13 +3129,13 @@
         <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3150,13 +3149,13 @@
         <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>57</v>
@@ -3168,13 +3167,13 @@
         <v>73</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -3188,7 +3187,7 @@
         <v>74</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>23</v>
@@ -3206,13 +3205,13 @@
         <v>73</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -3226,7 +3225,7 @@
         <v>74</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>58</v>
@@ -3241,13 +3240,13 @@
         <v>73</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -3261,7 +3260,7 @@
         <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>64</v>
@@ -3279,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3325,13 +3324,13 @@
         <v>73</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>74</v>
@@ -3340,7 +3339,7 @@
         <v>66</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3388,7 +3387,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -3403,7 +3402,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>75</v>
@@ -3417,7 +3416,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -3431,7 +3430,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>66</v>
@@ -3486,7 +3485,7 @@
         <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
@@ -3501,13 +3500,13 @@
         <v>73</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3521,7 +3520,7 @@
         <v>73</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>33</v>
@@ -3533,13 +3532,13 @@
         <v>73</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3553,7 +3552,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
@@ -3569,13 +3568,13 @@
         <v>73</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3589,7 +3588,7 @@
         <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>30</v>
@@ -3604,13 +3603,13 @@
         <v>73</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3656,13 +3655,13 @@
         <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>74</v>
@@ -3671,7 +3670,7 @@
         <v>66</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -3685,13 +3684,13 @@
         <v>74</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>74</v>
@@ -3700,7 +3699,7 @@
         <v>40</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3754,7 +3753,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -3789,7 +3788,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>75</v>
@@ -3806,7 +3805,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>28</v>
@@ -3820,7 +3819,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>66</v>
@@ -3878,10 +3877,10 @@
         <v>73</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>50</v>
@@ -3893,13 +3892,13 @@
         <v>73</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3913,7 +3912,7 @@
         <v>73</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>27</v>
@@ -3931,13 +3930,13 @@
         <v>73</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -3951,7 +3950,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -3966,13 +3965,13 @@
         <v>73</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -3986,7 +3985,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>23</v>
@@ -4001,13 +4000,13 @@
         <v>73</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -4021,7 +4020,7 @@
         <v>73</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
@@ -4036,13 +4035,13 @@
         <v>73</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -4056,7 +4055,7 @@
         <v>73</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>7</v>
@@ -4074,13 +4073,13 @@
         <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -4094,7 +4093,7 @@
         <v>74</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>23</v>
@@ -4109,16 +4108,16 @@
         <v>66</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -4132,25 +4131,25 @@
         <v>74</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -4164,7 +4163,7 @@
         <v>74</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>42</v>
@@ -4179,16 +4178,16 @@
         <v>28</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -4202,7 +4201,7 @@
         <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>23</v>
@@ -4211,7 +4210,7 @@
         <v>66</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J18" s="3">
         <v>0</v>
@@ -4234,7 +4233,7 @@
         <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>52</v>
@@ -4246,16 +4245,16 @@
         <v>28</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>73</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -4302,14 +4301,14 @@
         <v>73</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E22" t="s">
         <v>51</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>74</v>
@@ -4318,7 +4317,7 @@
         <v>66</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K22" s="2"/>
     </row>
@@ -4333,13 +4332,13 @@
         <v>74</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>74</v>
@@ -4348,7 +4347,7 @@
         <v>66</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L23" s="2"/>
     </row>
@@ -4363,16 +4362,16 @@
         <v>74</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>28</v>

</xml_diff>